<commit_message>
Update with Season 7 info
Season 7 new info except last episode's US viewers. Add stdev in main rating per season table and add text to last graph.
</commit_message>
<xml_diff>
--- a/rick_morty_imdb.xlsx
+++ b/rick_morty_imdb.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27218"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\DataScience\RickAndMorty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7F7232-BFC0-471A-8666-36E223F8835D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10C72662-9A98-48F1-8CF8-2851F66C1776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{392E6728-5297-46A7-A2E4-BF62F67AF9DD}"/>
   </bookViews>
   <sheets>
     <sheet name="imdb" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="206">
   <si>
     <t>season</t>
   </si>
@@ -49,6 +50,24 @@
     <t>name</t>
   </si>
   <si>
+    <t>directed_by</t>
+  </si>
+  <si>
+    <t>written_by</t>
+  </si>
+  <si>
+    <t>air_date</t>
+  </si>
+  <si>
+    <t>us_viewers_million</t>
+  </si>
+  <si>
+    <t>is_main_plot</t>
+  </si>
+  <si>
+    <t>is_referenced</t>
+  </si>
+  <si>
     <t>"Pilot"</t>
   </si>
   <si>
@@ -217,6 +236,9 @@
     <t>"Interdimensional Cable 2: Tempting Fate"</t>
   </si>
   <si>
+    <t>Dan Guterman, Ryan Ridley &amp; Justin Roiland</t>
+  </si>
+  <si>
     <t>September 20, 2015</t>
   </si>
   <si>
@@ -235,9 +257,6 @@
     <t>October 4, 2015</t>
   </si>
   <si>
-    <t>Dan Guterman, Ryan Ridley &amp; Justin Roiland</t>
-  </si>
-  <si>
     <t>"The Rickshank Rickdemption"</t>
   </si>
   <si>
@@ -286,6 +305,9 @@
     <t>August 27, 2017</t>
   </si>
   <si>
+    <t>"The Ricklantis Mixup"</t>
+  </si>
+  <si>
     <t>Dan Guterman &amp; Ryan Ridley</t>
   </si>
   <si>
@@ -295,6 +317,9 @@
     <t>"Morty's Mind Blowers"</t>
   </si>
   <si>
+    <t>Mike McMahan, James Siciliano, Ryan Ridley, Dan Guterman, Justin Roiland &amp; Dan Harmon</t>
+  </si>
+  <si>
     <t>September 17, 2017</t>
   </si>
   <si>
@@ -313,9 +338,6 @@
     <t>October 1, 2017</t>
   </si>
   <si>
-    <t>Mike McMahan, James Siciliano, Ryan Ridley, Dan Guterman, Justin Roiland &amp; Dan Harmon</t>
-  </si>
-  <si>
     <t>"Edge of Tomorty: Rick Die Rickpeat"</t>
   </si>
   <si>
@@ -493,98 +515,152 @@
     <t>September 4, 2022</t>
   </si>
   <si>
-    <t>directed_by</t>
-  </si>
-  <si>
-    <t>air_date</t>
-  </si>
-  <si>
-    <t>us_viewers_million</t>
-  </si>
-  <si>
-    <t>"The Ricklantis Mixup"</t>
-  </si>
-  <si>
-    <t>written_by</t>
-  </si>
-  <si>
-    <t>is_main_plot</t>
-  </si>
-  <si>
     <t>"Rick: A Mort Well Lived"</t>
   </si>
   <si>
+    <t>September 11, 2022</t>
+  </si>
+  <si>
     <t>"Bethic Twinstinct"</t>
   </si>
   <si>
+    <t>Douglas Einar Olsen</t>
+  </si>
+  <si>
+    <t>September 18, 2022</t>
+  </si>
+  <si>
     <t>"Night Family"</t>
   </si>
   <si>
+    <t>September 25, 2022</t>
+  </si>
+  <si>
     <t>"Final DeSmithation"</t>
   </si>
   <si>
+    <t>Heather Anne Campbell</t>
+  </si>
+  <si>
+    <t>October 2, 2022</t>
+  </si>
+  <si>
     <t>"Juricksic Mort"</t>
   </si>
   <si>
-    <t>Douglas Einar Olsen</t>
-  </si>
-  <si>
-    <t>Heather Anne Campbell</t>
-  </si>
-  <si>
     <t>October 9, 2022</t>
   </si>
   <si>
-    <t>October 2, 2022</t>
-  </si>
-  <si>
-    <t>September 25, 2022</t>
-  </si>
-  <si>
-    <t>September 18, 2022</t>
-  </si>
-  <si>
-    <t>September 11, 2022</t>
-  </si>
-  <si>
     <t>"Full Meta Jackrick"</t>
   </si>
   <si>
+    <t>November 20, 2022</t>
+  </si>
+  <si>
     <t>"Analyze Piss"</t>
   </si>
   <si>
+    <t>Fill Marc Sagadraca</t>
+  </si>
+  <si>
+    <t>November 27, 2022</t>
+  </si>
+  <si>
     <t>"A Rick in King Mortur's Mort"</t>
   </si>
   <si>
+    <t>December 4, 2022</t>
+  </si>
+  <si>
     <t>"Ricktional Mortpoon's Rickmas Mortcation"</t>
   </si>
   <si>
-    <t>November 20, 2022</t>
-  </si>
-  <si>
-    <t>is_referenced</t>
-  </si>
-  <si>
-    <t>Fill Marc Sagadraca</t>
-  </si>
-  <si>
-    <t>November 27, 2022</t>
-  </si>
-  <si>
-    <t>December 4, 2022</t>
-  </si>
-  <si>
     <t>Scott Marder</t>
   </si>
   <si>
     <t>December 11, 2022</t>
+  </si>
+  <si>
+    <t>How Poopy Got His Poop Back</t>
+  </si>
+  <si>
+    <t>October 15, 2023</t>
+  </si>
+  <si>
+    <t>The Jerrick Trap</t>
+  </si>
+  <si>
+    <t>Albro Lundy &amp; James Siciliano</t>
+  </si>
+  <si>
+    <t>October 22, 2023</t>
+  </si>
+  <si>
+    <t>Air Force Wong</t>
+  </si>
+  <si>
+    <t>October 29, 2023</t>
+  </si>
+  <si>
+    <t>That's Amorte</t>
+  </si>
+  <si>
+    <t>November 5, 2023</t>
+  </si>
+  <si>
+    <t>Unmortricken</t>
+  </si>
+  <si>
+    <t>November 12, 2023</t>
+  </si>
+  <si>
+    <t>Rickfending Your Mort</t>
+  </si>
+  <si>
+    <t>Cody Ziglar</t>
+  </si>
+  <si>
+    <t>November 19, 2023</t>
+  </si>
+  <si>
+    <t>Wet Kuat Amortican Summer</t>
+  </si>
+  <si>
+    <t>Alex Song-Xia</t>
+  </si>
+  <si>
+    <t>November 26, 2023</t>
+  </si>
+  <si>
+    <t>Rise of the Numbericons: The Movie</t>
+  </si>
+  <si>
+    <t>December 3, 2023</t>
+  </si>
+  <si>
+    <t>Mort: Ragnarick</t>
+  </si>
+  <si>
+    <t>Jeremy Gilfor &amp; Scott Marder</t>
+  </si>
+  <si>
+    <t>December 10, 2023</t>
+  </si>
+  <si>
+    <t>Fear No Mort</t>
+  </si>
+  <si>
+    <t>Eugene Huang</t>
+  </si>
+  <si>
+    <t>December 17, 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,16 +668,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -609,12 +697,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA2A9B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,13 +1036,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6C67F3-F0A8-4121-8F2C-FB09D8345F03}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -944,9 +1052,10 @@
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="82.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,25 +1069,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -989,16 +1098,16 @@
         <v>7.9</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>1.1000000000000001</v>
@@ -1007,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1018,16 +1127,16 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H3">
         <v>1.51</v>
@@ -1036,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1047,16 +1156,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>1.3</v>
@@ -1065,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1076,16 +1185,16 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H5">
         <v>1.32</v>
@@ -1094,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1105,16 +1214,16 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>1.61</v>
@@ -1123,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1134,16 +1243,16 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <v>1.75</v>
@@ -1152,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1163,16 +1272,16 @@
         <v>7.9</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H8">
         <v>1.76</v>
@@ -1181,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1192,16 +1301,16 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H9">
         <v>1.48</v>
@@ -1210,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1221,16 +1330,16 @@
         <v>8.4</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H10">
         <v>1.54</v>
@@ -1239,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1250,16 +1359,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H11">
         <v>1.75</v>
@@ -1268,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1279,16 +1388,16 @@
         <v>8.4</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H12">
         <v>2.13</v>
@@ -1297,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1308,16 +1417,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H13">
         <v>2.12</v>
@@ -1326,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1337,16 +1446,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="H14">
         <v>2.19</v>
@@ -1355,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1366,16 +1475,16 @@
         <v>8.5</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H15">
         <v>1.94</v>
@@ -1384,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1395,16 +1504,16 @@
         <v>9.5</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H16">
         <v>1.96</v>
@@ -1413,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1424,16 +1533,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H17">
         <v>2.12</v>
@@ -1442,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1453,16 +1562,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H18">
         <v>1.91</v>
@@ -1471,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1482,16 +1591,16 @@
         <v>8.4</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H19">
         <v>1.97</v>
@@ -1500,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1511,16 +1620,16 @@
         <v>7.6</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
         <v>66</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H20">
         <v>1.79</v>
@@ -1529,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1540,16 +1649,16 @@
         <v>8.5</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H21">
         <v>1.89</v>
@@ -1558,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1569,16 +1678,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="H22">
         <v>1.84</v>
@@ -1587,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1598,16 +1707,16 @@
         <v>9.6</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H23">
         <v>0.68</v>
@@ -1616,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1627,16 +1736,16 @@
         <v>8.1</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H24">
         <v>2.86</v>
@@ -1645,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1656,16 +1765,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H25">
         <v>2.31</v>
@@ -1674,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1685,16 +1794,16 @@
         <v>8.1</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H26">
         <v>2.66</v>
@@ -1703,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1714,16 +1823,16 @@
         <v>8.4</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H27">
         <v>2.29</v>
@@ -1732,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1743,16 +1852,16 @@
         <v>8.9</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="H28">
         <v>2.4700000000000002</v>
@@ -1761,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1772,16 +1881,16 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H29">
         <v>2.38</v>
@@ -1790,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1801,16 +1910,16 @@
         <v>8.9</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="H30">
         <v>2.5099999999999998</v>
@@ -1819,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1830,16 +1939,16 @@
         <v>8.9</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="H31">
         <v>2.4900000000000002</v>
@@ -1848,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1859,16 +1968,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H32">
         <v>2.6</v>
@@ -1877,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1888,16 +1997,16 @@
         <v>8.9</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E33" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="H33">
         <v>2.33</v>
@@ -1906,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1917,16 +2026,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E34" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="G34" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="H34">
         <v>1.67</v>
@@ -1935,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1946,16 +2055,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F35" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="H35">
         <v>1.61</v>
@@ -1964,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1975,16 +2084,16 @@
         <v>7.3</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F36" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G36" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="H36">
         <v>1.63</v>
@@ -1993,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2004,16 +2113,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D37" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F37" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G37" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="H37">
         <v>1.32</v>
@@ -2022,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2033,16 +2142,16 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G38" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="H38">
         <v>1.55</v>
@@ -2051,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2062,16 +2171,16 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
         <v>111</v>
       </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" t="s">
-        <v>104</v>
-      </c>
       <c r="G39" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="H39">
         <v>1.34</v>
@@ -2080,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2091,16 +2200,16 @@
         <v>9.4</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E40" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F40" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G40" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H40">
         <v>1.26</v>
@@ -2109,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2120,16 +2229,16 @@
         <v>7.7</v>
       </c>
       <c r="D41" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F41" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G41" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H41">
         <v>1.22</v>
@@ -2138,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2149,16 +2258,16 @@
         <v>9.1</v>
       </c>
       <c r="D42" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F42" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G42" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H42">
         <v>1.3</v>
@@ -2167,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2178,16 +2287,16 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E43" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F43" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G43" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H43">
         <v>1.3</v>
@@ -2196,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2207,16 +2316,16 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E44" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F44" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G44" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="H44">
         <v>1.1599999999999999</v>
@@ -2225,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2236,16 +2345,16 @@
         <v>7.8</v>
       </c>
       <c r="D45" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E45" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="F45" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="G45" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H45">
         <v>1.01</v>
@@ -2254,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2265,16 +2374,16 @@
         <v>5.7</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G46" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="H46">
         <v>0.96</v>
@@ -2283,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2294,16 +2403,16 @@
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="E47" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F47" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G47" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="H47">
         <v>0.78</v>
@@ -2312,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>5</v>
       </c>
@@ -2323,16 +2432,16 @@
         <v>7.1</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E48" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F48" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G48" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="H48">
         <v>0.93</v>
@@ -2341,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>5</v>
       </c>
@@ -2352,16 +2461,16 @@
         <v>6.4</v>
       </c>
       <c r="D49" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E49" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="H49">
         <v>0.82</v>
@@ -2370,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2381,16 +2490,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F50" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G50" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H50">
         <v>0.83</v>
@@ -2399,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2410,16 +2519,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E51" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F51" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G51" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H51">
         <v>0.91</v>
@@ -2428,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2439,16 +2548,16 @@
         <v>9.4</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F52" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="G52" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H52">
         <v>0.94</v>
@@ -2457,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2468,16 +2577,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D53" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E53" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F53" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G53" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="H53">
         <v>0.66</v>
@@ -2486,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2497,16 +2606,16 @@
         <v>7.9</v>
       </c>
       <c r="D54" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E54" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F54" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G54" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H54">
         <v>0.6</v>
@@ -2515,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2526,16 +2635,16 @@
         <v>7.8</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E55" t="s">
+        <v>162</v>
+      </c>
+      <c r="F55" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" t="s">
         <v>163</v>
-      </c>
-      <c r="F55" t="s">
-        <v>120</v>
-      </c>
-      <c r="G55" t="s">
-        <v>168</v>
       </c>
       <c r="H55">
         <v>0.55000000000000004</v>
@@ -2544,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>6</v>
       </c>
@@ -2555,16 +2664,16 @@
         <v>8.6</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E56" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F56" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="G56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H56">
         <v>0.6</v>
@@ -2573,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>6</v>
       </c>
@@ -2584,16 +2693,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D57" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F57" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G57" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H57">
         <v>0.57999999999999996</v>
@@ -2602,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>6</v>
       </c>
@@ -2613,16 +2722,16 @@
         <v>8.1</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E58" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F58" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G58" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H58">
         <v>0.54</v>
@@ -2631,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2642,16 +2751,16 @@
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F59" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G59" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H59">
         <v>0.51</v>
@@ -2660,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>6</v>
       </c>
@@ -2671,16 +2780,16 @@
         <v>8.4</v>
       </c>
       <c r="D60" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E60" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F60" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G60" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H60">
         <v>0.53</v>
@@ -2692,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>6</v>
       </c>
@@ -2703,16 +2812,16 @@
         <v>7.6</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E61" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F61" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H61">
         <v>0.53</v>
@@ -2724,7 +2833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>6</v>
       </c>
@@ -2735,10 +2844,10 @@
         <v>8.1</v>
       </c>
       <c r="D62" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E62" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F62" t="s">
         <v>179</v>
@@ -2753,6 +2862,293 @@
         <v>1</v>
       </c>
       <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63">
+        <v>7</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" t="s">
+        <v>132</v>
+      </c>
+      <c r="F63" t="s">
+        <v>140</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H63">
+        <v>0.42</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64">
+        <v>7</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>7.4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>183</v>
+      </c>
+      <c r="E64" t="s">
+        <v>124</v>
+      </c>
+      <c r="F64" t="s">
+        <v>184</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H64">
+        <v>0.47</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65">
+        <v>7</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>6.8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>186</v>
+      </c>
+      <c r="E65" t="s">
+        <v>104</v>
+      </c>
+      <c r="F65" t="s">
+        <v>63</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H65">
+        <v>0.36</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="28.5">
+      <c r="A66">
+        <v>7</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D66" t="s">
+        <v>188</v>
+      </c>
+      <c r="E66" t="s">
+        <v>132</v>
+      </c>
+      <c r="F66" t="s">
+        <v>167</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H66">
+        <v>0.44</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.5">
+      <c r="A67">
+        <v>7</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D67" t="s">
+        <v>190</v>
+      </c>
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" t="s">
+        <v>184</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H67">
+        <v>0.46</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="28.5">
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>192</v>
+      </c>
+      <c r="E68" t="s">
+        <v>104</v>
+      </c>
+      <c r="F68" t="s">
+        <v>193</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H68">
+        <v>0.4</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="28.5">
+      <c r="A69">
+        <v>7</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>6.5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>195</v>
+      </c>
+      <c r="E69" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" t="s">
+        <v>196</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H69">
+        <v>0.49</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="28.5">
+      <c r="A70">
+        <v>7</v>
+      </c>
+      <c r="B70">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D70" t="s">
+        <v>198</v>
+      </c>
+      <c r="E70" t="s">
+        <v>132</v>
+      </c>
+      <c r="F70" t="s">
+        <v>137</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H70">
+        <v>0.38</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="28.5">
+      <c r="A71">
+        <v>7</v>
+      </c>
+      <c r="B71">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>200</v>
+      </c>
+      <c r="E71" t="s">
+        <v>124</v>
+      </c>
+      <c r="F71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H71">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="28.5">
+      <c r="A72">
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>9.4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>203</v>
+      </c>
+      <c r="E72" t="s">
+        <v>204</v>
+      </c>
+      <c r="F72" t="s">
+        <v>167</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I72">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Season 8 info
Update Season 8 info
Revisits IMDB rankings for previous seasons.
FIX: score of episode Bethic Twinstinct
</commit_message>
<xml_diff>
--- a/rick_morty_imdb.xlsx
+++ b/rick_morty_imdb.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27218"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\DataScience\RickAndMorty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10C72662-9A98-48F1-8CF8-2851F66C1776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37FAA94E-03D3-46DE-BFA1-9C76D27CC0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{392E6728-5297-46A7-A2E4-BF62F67AF9DD}"/>
   </bookViews>
   <sheets>
     <sheet name="imdb" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="266">
   <si>
     <t>season</t>
   </si>
@@ -68,7 +69,10 @@
     <t>is_referenced</t>
   </si>
   <si>
-    <t>"Pilot"</t>
+    <t>is_citadel</t>
+  </si>
+  <si>
+    <t>Pilot</t>
   </si>
   <si>
     <t>Justin Roiland</t>
@@ -80,7 +84,7 @@
     <t>December 2, 2013</t>
   </si>
   <si>
-    <t>"Lawnmower Dog"</t>
+    <t>Lawnmower Dog</t>
   </si>
   <si>
     <t>John Rice</t>
@@ -92,7 +96,7 @@
     <t>December 9, 2013</t>
   </si>
   <si>
-    <t>"Anatomy Park"</t>
+    <t>Anatomy Park</t>
   </si>
   <si>
     <t>Eric Acosta &amp; Wade Randolph</t>
@@ -101,7 +105,7 @@
     <t>December 16, 2013</t>
   </si>
   <si>
-    <t>"M. Night Shaym-Aliens!"</t>
+    <t>M. Night Shaym-Aliens!</t>
   </si>
   <si>
     <t>Jeff Myers</t>
@@ -113,7 +117,7 @@
     <t>January 13, 2014</t>
   </si>
   <si>
-    <t>"Meeseeks and Destroy"</t>
+    <t>Meeseeks and Destroy</t>
   </si>
   <si>
     <t>Bryan Newton</t>
@@ -122,7 +126,7 @@
     <t>January 20, 2014</t>
   </si>
   <si>
-    <t>"Rick Potion #9"</t>
+    <t>Rick Potion #9</t>
   </si>
   <si>
     <t>Stephen Sandoval</t>
@@ -131,13 +135,13 @@
     <t>January 27, 2014</t>
   </si>
   <si>
-    <t>"Raising Gazorpazorp"</t>
+    <t>Raising Gazorpazorp</t>
   </si>
   <si>
     <t>March 10, 2014</t>
   </si>
   <si>
-    <t>"Rixty Minutes"</t>
+    <t>Rixty Minutes</t>
   </si>
   <si>
     <t>Tom Kauffman &amp; Justin Roiland</t>
@@ -146,7 +150,7 @@
     <t>March 17, 2014</t>
   </si>
   <si>
-    <t>"Something Ricked This Way Comes"</t>
+    <t>Something Ricked This Way Comes</t>
   </si>
   <si>
     <t>Mike McMahan</t>
@@ -155,13 +159,13 @@
     <t>March 24, 2014</t>
   </si>
   <si>
-    <t>"Close Rick-counters of the Rick Kind"</t>
+    <t>Close Rick-counters of the Rick Kind</t>
   </si>
   <si>
     <t>April 7, 2014</t>
   </si>
   <si>
-    <t>"Ricksy Business"</t>
+    <t>Ricksy Business</t>
   </si>
   <si>
     <t>Ryan Ridley &amp; Tom Kauffman</t>
@@ -170,7 +174,7 @@
     <t>April 14, 2014</t>
   </si>
   <si>
-    <t>"A Rickle in Time"</t>
+    <t>A Rickle in Time</t>
   </si>
   <si>
     <t>Wes Archer</t>
@@ -182,7 +186,7 @@
     <t>July 26, 2015</t>
   </si>
   <si>
-    <t>"Mortynight Run"</t>
+    <t>Mortynight Run</t>
   </si>
   <si>
     <t>Dominic Polcino</t>
@@ -194,13 +198,13 @@
     <t>August 2, 2015</t>
   </si>
   <si>
-    <t>"Auto Erotic Assimilation"</t>
+    <t>Auto Erotic Assimilation</t>
   </si>
   <si>
     <t>August 9, 2015</t>
   </si>
   <si>
-    <t>"Total Rickall"</t>
+    <t>Total Rickall</t>
   </si>
   <si>
     <t>Juan Meza-León</t>
@@ -209,13 +213,13 @@
     <t>August 16, 2015</t>
   </si>
   <si>
-    <t>"Get Schwifty"</t>
+    <t>Get Schwifty</t>
   </si>
   <si>
     <t>August 23, 2015</t>
   </si>
   <si>
-    <t>"The Ricks Must Be Crazy"</t>
+    <t>The Ricks Must Be Crazy</t>
   </si>
   <si>
     <t>Dan Guterman</t>
@@ -224,7 +228,7 @@
     <t>August 30, 2015</t>
   </si>
   <si>
-    <t>"Big Trouble in Little Sanchez"</t>
+    <t>Big Trouble in Little Sanchez</t>
   </si>
   <si>
     <t>Alex Rubens</t>
@@ -233,7 +237,7 @@
     <t>September 13, 2015</t>
   </si>
   <si>
-    <t>"Interdimensional Cable 2: Tempting Fate"</t>
+    <t>Interdimensional Cable 2: Tempting Fate</t>
   </si>
   <si>
     <t>Dan Guterman, Ryan Ridley &amp; Justin Roiland</t>
@@ -242,7 +246,7 @@
     <t>September 20, 2015</t>
   </si>
   <si>
-    <t>"Look Who's Purging Now"</t>
+    <t>Look Who's Purging Now</t>
   </si>
   <si>
     <t>Dan Harmon, Ryan Ridley &amp; Justin Roiland</t>
@@ -251,19 +255,19 @@
     <t>September 27, 2015</t>
   </si>
   <si>
-    <t>"The Wedding Squanchers"</t>
+    <t>The Wedding Squanchers</t>
   </si>
   <si>
     <t>October 4, 2015</t>
   </si>
   <si>
-    <t>"The Rickshank Rickdemption"</t>
+    <t>The Rickshank Rickdemption</t>
   </si>
   <si>
     <t>April 1, 2017</t>
   </si>
   <si>
-    <t>"Rickmancing the Stone"</t>
+    <t>Rickmancing the Stone</t>
   </si>
   <si>
     <t>Jane Becker</t>
@@ -272,7 +276,7 @@
     <t>July 30, 2017</t>
   </si>
   <si>
-    <t>"Pickle Rick"</t>
+    <t>Pickle Rick</t>
   </si>
   <si>
     <t>Anthony Chun</t>
@@ -284,7 +288,7 @@
     <t>August 6, 2017</t>
   </si>
   <si>
-    <t>"Vindicators 3: The Return of Worldender"</t>
+    <t>Vindicators 3: The Return of Worldender</t>
   </si>
   <si>
     <t>Sarah Carbiener &amp; Erica Rosbe</t>
@@ -293,19 +297,19 @@
     <t>August 13, 2017</t>
   </si>
   <si>
-    <t>"The Whirly Dirly Conspiracy"</t>
+    <t>The Whirly Dirly Conspiracy</t>
   </si>
   <si>
     <t>August 20, 2017</t>
   </si>
   <si>
-    <t>"Rest and Ricklaxation"</t>
+    <t>Rest and Ricklaxation</t>
   </si>
   <si>
     <t>August 27, 2017</t>
   </si>
   <si>
-    <t>"The Ricklantis Mixup"</t>
+    <t>The Ricklantis Mixup</t>
   </si>
   <si>
     <t>Dan Guterman &amp; Ryan Ridley</t>
@@ -314,7 +318,7 @@
     <t>September 10, 2017</t>
   </si>
   <si>
-    <t>"Morty's Mind Blowers"</t>
+    <t>Morty's Mind Blowers</t>
   </si>
   <si>
     <t>Mike McMahan, James Siciliano, Ryan Ridley, Dan Guterman, Justin Roiland &amp; Dan Harmon</t>
@@ -323,13 +327,13 @@
     <t>September 17, 2017</t>
   </si>
   <si>
-    <t>"The ABC's of Beth"</t>
+    <t>The ABC's of Beth</t>
   </si>
   <si>
     <t>September 24, 2017</t>
   </si>
   <si>
-    <t>"The Rickchurian Mortydate"</t>
+    <t>The Rickchurian Mortydate</t>
   </si>
   <si>
     <t>Dan Harmon</t>
@@ -338,7 +342,7 @@
     <t>October 1, 2017</t>
   </si>
   <si>
-    <t>"Edge of Tomorty: Rick Die Rickpeat"</t>
+    <t>Edge of Tomorty: Rick Die Rickpeat</t>
   </si>
   <si>
     <t>Erica Hayes</t>
@@ -347,7 +351,7 @@
     <t>November 10, 2019</t>
   </si>
   <si>
-    <t>"The Old Man and the Seat"</t>
+    <t>The Old Man and the Seat</t>
   </si>
   <si>
     <t>Jacob Hair</t>
@@ -359,7 +363,7 @@
     <t>November 17, 2019</t>
   </si>
   <si>
-    <t>"One Crew over the Crewcoo's Morty"</t>
+    <t>One Crew over the Crewcoo's Morty</t>
   </si>
   <si>
     <t>Caitie Delaney</t>
@@ -368,7 +372,7 @@
     <t>November 24, 2019</t>
   </si>
   <si>
-    <t>"Claw and Hoarder: Special Ricktim's Morty"</t>
+    <t>Claw and Hoarder: Special Ricktim's Morty</t>
   </si>
   <si>
     <t>Jeff Loveness</t>
@@ -377,7 +381,7 @@
     <t>December 8, 2019</t>
   </si>
   <si>
-    <t>"Rattlestar Ricklactica"</t>
+    <t>Rattlestar Ricklactica</t>
   </si>
   <si>
     <t>James Siciliano</t>
@@ -386,19 +390,19 @@
     <t>December 15, 2019</t>
   </si>
   <si>
-    <t>"Never Ricking Morty"</t>
+    <t>Never Ricking Morty</t>
   </si>
   <si>
     <t>May 3, 2020</t>
   </si>
   <si>
-    <t>"Promortyus"</t>
+    <t>Promortyus</t>
   </si>
   <si>
     <t>May 10, 2020</t>
   </si>
   <si>
-    <t>"The Vat of Acid Episode"</t>
+    <t>The Vat of Acid Episode</t>
   </si>
   <si>
     <t>Jeff Loveness &amp; Albro Lundy</t>
@@ -407,7 +411,7 @@
     <t>May 17, 2020</t>
   </si>
   <si>
-    <t>"Childrick of Mort"</t>
+    <t>Childrick of Mort</t>
   </si>
   <si>
     <t>Kyounghee Lim</t>
@@ -416,7 +420,7 @@
     <t>May 24, 2020</t>
   </si>
   <si>
-    <t>"Star Mort Rickturn of the Jerri"</t>
+    <t>Star Mort Rickturn of the Jerri</t>
   </si>
   <si>
     <t>Anne Lane</t>
@@ -425,13 +429,13 @@
     <t>May 31, 2020</t>
   </si>
   <si>
-    <t>"Mort Dinner Rick Andre"</t>
+    <t>Mort Dinner Rick Andre</t>
   </si>
   <si>
     <t>June 20, 2021</t>
   </si>
   <si>
-    <t>"Mortyplicity"</t>
+    <t>Mortyplicity</t>
   </si>
   <si>
     <t>Lucas Gray</t>
@@ -443,7 +447,7 @@
     <t>June 27, 2021</t>
   </si>
   <si>
-    <t>"A Rickconvenient Mort"</t>
+    <t>A Rickconvenient Mort</t>
   </si>
   <si>
     <t>Juan Meza-Léon</t>
@@ -455,7 +459,7 @@
     <t>July 4, 2021</t>
   </si>
   <si>
-    <t>"Rickdependence Spray"</t>
+    <t>Rickdependence Spray</t>
   </si>
   <si>
     <t>Nick Rutherford</t>
@@ -464,13 +468,13 @@
     <t>July 11, 2021</t>
   </si>
   <si>
-    <t>"Amortycan Grickfitti"</t>
+    <t>Amortycan Grickfitti</t>
   </si>
   <si>
     <t>July 18, 2021</t>
   </si>
   <si>
-    <t>"Rick &amp; Morty's Thanksploitation Spectacular"</t>
+    <t>Rick &amp; Morty's Thanksploitation Spectacular</t>
   </si>
   <si>
     <t>Douglas Olsen</t>
@@ -479,7 +483,7 @@
     <t>July 25, 2021</t>
   </si>
   <si>
-    <t>"Gotron Jerrysis Rickvangelion"</t>
+    <t>Gotron Jerrysis Rickvangelion</t>
   </si>
   <si>
     <t>John Harris</t>
@@ -488,13 +492,13 @@
     <t>August 1, 2021[d]</t>
   </si>
   <si>
-    <t>"Rickternal Friendshine of the Spotless Mort"</t>
+    <t>Rickternal Friendshine of the Spotless Mort</t>
   </si>
   <si>
     <t>August 8, 2021</t>
   </si>
   <si>
-    <t>"Forgetting Sarick Mortshall"</t>
+    <t>Forgetting Sarick Mortshall</t>
   </si>
   <si>
     <t>Siobhan Thompson</t>
@@ -503,25 +507,25 @@
     <t>September 5, 2021</t>
   </si>
   <si>
-    <t>"Rickmurai Jack"</t>
+    <t>Rickmurai Jack</t>
   </si>
   <si>
     <t>Jeff Loveness &amp; Scott Marder</t>
   </si>
   <si>
-    <t>"Solaricks"</t>
+    <t>Solaricks</t>
   </si>
   <si>
     <t>September 4, 2022</t>
   </si>
   <si>
-    <t>"Rick: A Mort Well Lived"</t>
+    <t>Rick: A Mort Well Lived</t>
   </si>
   <si>
     <t>September 11, 2022</t>
   </si>
   <si>
-    <t>"Bethic Twinstinct"</t>
+    <t>Bethic Twinstinct</t>
   </si>
   <si>
     <t>Douglas Einar Olsen</t>
@@ -530,13 +534,13 @@
     <t>September 18, 2022</t>
   </si>
   <si>
-    <t>"Night Family"</t>
+    <t>Night Family</t>
   </si>
   <si>
     <t>September 25, 2022</t>
   </si>
   <si>
-    <t>"Final DeSmithation"</t>
+    <t>Final DeSmithation</t>
   </si>
   <si>
     <t>Heather Anne Campbell</t>
@@ -545,19 +549,19 @@
     <t>October 2, 2022</t>
   </si>
   <si>
-    <t>"Juricksic Mort"</t>
+    <t>Juricksic Mort</t>
   </si>
   <si>
     <t>October 9, 2022</t>
   </si>
   <si>
-    <t>"Full Meta Jackrick"</t>
+    <t>Full Meta Jackrick</t>
   </si>
   <si>
     <t>November 20, 2022</t>
   </si>
   <si>
-    <t>"Analyze Piss"</t>
+    <t>Analyze Piss</t>
   </si>
   <si>
     <t>Fill Marc Sagadraca</t>
@@ -566,13 +570,13 @@
     <t>November 27, 2022</t>
   </si>
   <si>
-    <t>"A Rick in King Mortur's Mort"</t>
+    <t>A Rick in King Mortur's Mort</t>
   </si>
   <si>
     <t>December 4, 2022</t>
   </si>
   <si>
-    <t>"Ricktional Mortpoon's Rickmas Mortcation"</t>
+    <t>Ricktional Mortpoon's Rickmas Mortcation</t>
   </si>
   <si>
     <t>Scott Marder</t>
@@ -654,13 +658,194 @@
   </si>
   <si>
     <t>December 17, 2023</t>
+  </si>
+  <si>
+    <t>Summer of All Fears</t>
+  </si>
+  <si>
+    <t>Jess Lacher</t>
+  </si>
+  <si>
+    <t>May 25, 2025</t>
+  </si>
+  <si>
+    <t>Valkyrick</t>
+  </si>
+  <si>
+    <t>June 1, 2025</t>
+  </si>
+  <si>
+    <t>The Rick, The Mort &amp; The Ugly</t>
+  </si>
+  <si>
+    <t>Brian Kaufman</t>
+  </si>
+  <si>
+    <t>Albro Lundy, James Siciliano &amp; Michael Kellner</t>
+  </si>
+  <si>
+    <t>June 8, 2025</t>
+  </si>
+  <si>
+    <t>The Last Temptation of Jerry</t>
+  </si>
+  <si>
+    <t>June 15, 2025</t>
+  </si>
+  <si>
+    <t>Cryo Mort a Rickver</t>
+  </si>
+  <si>
+    <t>June 22, 2025</t>
+  </si>
+  <si>
+    <t>The Curicksous Case of Bethjamin Button</t>
+  </si>
+  <si>
+    <t>Heather Anne Campbell &amp; Jess Lacher</t>
+  </si>
+  <si>
+    <t>June 29, 2025</t>
+  </si>
+  <si>
+    <t>Ricker than Fiction</t>
+  </si>
+  <si>
+    <t>July 6, 2025</t>
+  </si>
+  <si>
+    <t>Nomortland</t>
+  </si>
+  <si>
+    <t>July 13, 2025</t>
+  </si>
+  <si>
+    <t>Morty Daddy</t>
+  </si>
+  <si>
+    <t>Beth Stelling</t>
+  </si>
+  <si>
+    <t>July 20, 2025</t>
+  </si>
+  <si>
+    <t>Hot Rick</t>
+  </si>
+  <si>
+    <t>July 27, 2025</t>
+  </si>
+  <si>
+    <t>No.
+overall</t>
+  </si>
+  <si>
+    <t>No. in
+season</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Directed by</t>
+  </si>
+  <si>
+    <t>Written by</t>
+  </si>
+  <si>
+    <t>Original release date [7]</t>
+  </si>
+  <si>
+    <t>Prod.
+code [29]</t>
+  </si>
+  <si>
+    <t>U.S. viewers
+(millions)</t>
+  </si>
+  <si>
+    <t>"Summer of All Fears"</t>
+  </si>
+  <si>
+    <t>RAM-801</t>
+  </si>
+  <si>
+    <t>0.30[82]</t>
+  </si>
+  <si>
+    <t>"Valkyrick"</t>
+  </si>
+  <si>
+    <t>RAM-802</t>
+  </si>
+  <si>
+    <t>0.47[83]</t>
+  </si>
+  <si>
+    <t>"The Rick, The Mort &amp; The Ugly"</t>
+  </si>
+  <si>
+    <t>RAM-803</t>
+  </si>
+  <si>
+    <t>0.33[84]</t>
+  </si>
+  <si>
+    <t>"The Last Temptation of Jerry"</t>
+  </si>
+  <si>
+    <t>RAM-804</t>
+  </si>
+  <si>
+    <t>0.38[85]</t>
+  </si>
+  <si>
+    <t>"Cryo Mort a Rickver"</t>
+  </si>
+  <si>
+    <t>RAM-805</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>"The Curicksous Case of Bethjamin Button"</t>
+  </si>
+  <si>
+    <t>RAM-806</t>
+  </si>
+  <si>
+    <t>"Ricker than Fiction"</t>
+  </si>
+  <si>
+    <t>RAM-807</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>"Nomortland"</t>
+  </si>
+  <si>
+    <t>RAM-808</t>
+  </si>
+  <si>
+    <t>"Morty Daddy"</t>
+  </si>
+  <si>
+    <t>RAM-809</t>
+  </si>
+  <si>
+    <t>"Hot Rick"</t>
+  </si>
+  <si>
+    <t>RAM-810</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,13 +854,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF202122"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2C2C2C"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,7 +890,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FF2F5E73"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAECF0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -713,17 +931,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1036,11 +1270,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6C67F3-F0A8-4121-8F2C-FB09D8345F03}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I67" sqref="I67"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1050,12 +1284,12 @@
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="82.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
     <col min="7" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1086,8 +1320,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1098,16 +1335,16 @@
         <v>7.9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>1.1000000000000001</v>
@@ -1115,8 +1352,11 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1124,19 +1364,19 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>8.6999999999999993</v>
+        <v>8.6</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>1.51</v>
@@ -1144,8 +1384,11 @@
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1156,16 +1399,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4">
         <v>1.3</v>
@@ -1173,8 +1416,11 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1182,19 +1428,19 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>8.6999999999999993</v>
+        <v>8.6</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>1.32</v>
@@ -1202,8 +1448,11 @@
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1214,16 +1463,16 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6">
         <v>1.61</v>
@@ -1231,8 +1480,11 @@
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1240,19 +1492,19 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7">
         <v>1.75</v>
@@ -1260,8 +1512,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1272,16 +1527,16 @@
         <v>7.9</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <v>1.76</v>
@@ -1289,8 +1544,11 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1298,19 +1556,19 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>8.6999999999999993</v>
+        <v>8.6</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H9">
         <v>1.48</v>
@@ -1318,8 +1576,11 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1330,16 +1591,16 @@
         <v>8.4</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10">
         <v>1.54</v>
@@ -1347,8 +1608,11 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1359,16 +1623,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H11">
         <v>1.75</v>
@@ -1376,8 +1640,11 @@
       <c r="I11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1388,16 +1655,16 @@
         <v>8.4</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H12">
         <v>2.13</v>
@@ -1405,8 +1672,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1417,16 +1687,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H13">
         <v>2.12</v>
@@ -1434,8 +1704,11 @@
       <c r="I13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1446,16 +1719,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H14">
         <v>2.19</v>
@@ -1463,8 +1736,11 @@
       <c r="I14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1475,16 +1751,16 @@
         <v>8.5</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H15">
         <v>1.94</v>
@@ -1492,8 +1768,11 @@
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1504,16 +1783,16 @@
         <v>9.5</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H16">
         <v>1.96</v>
@@ -1521,8 +1800,11 @@
       <c r="I16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1533,16 +1815,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H17">
         <v>2.12</v>
@@ -1550,8 +1832,11 @@
       <c r="I17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1562,16 +1847,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18">
         <v>1.91</v>
@@ -1579,8 +1864,11 @@
       <c r="I18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1591,16 +1879,16 @@
         <v>8.4</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H19">
         <v>1.97</v>
@@ -1608,8 +1896,11 @@
       <c r="I19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1620,16 +1911,16 @@
         <v>7.6</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H20">
         <v>1.79</v>
@@ -1637,8 +1928,11 @@
       <c r="I20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1649,16 +1943,16 @@
         <v>8.5</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H21">
         <v>1.89</v>
@@ -1666,8 +1960,11 @@
       <c r="I21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1678,16 +1975,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H22">
         <v>1.84</v>
@@ -1695,8 +1992,11 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1707,16 +2007,16 @@
         <v>9.6</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>0.68</v>
@@ -1724,8 +2024,11 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1736,16 +2039,16 @@
         <v>8.1</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H24">
         <v>2.86</v>
@@ -1753,8 +2056,11 @@
       <c r="I24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1765,16 +2071,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H25">
         <v>2.31</v>
@@ -1782,8 +2088,11 @@
       <c r="I25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1794,16 +2103,16 @@
         <v>8.1</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H26">
         <v>2.66</v>
@@ -1811,8 +2120,11 @@
       <c r="I26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1823,16 +2135,16 @@
         <v>8.4</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H27">
         <v>2.29</v>
@@ -1840,8 +2152,11 @@
       <c r="I27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1849,19 +2164,19 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>8.9</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H28">
         <v>2.4700000000000002</v>
@@ -1869,8 +2184,11 @@
       <c r="I28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1881,16 +2199,16 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H29">
         <v>2.38</v>
@@ -1898,8 +2216,11 @@
       <c r="I29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1910,16 +2231,16 @@
         <v>8.9</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H30">
         <v>2.5099999999999998</v>
@@ -1927,8 +2248,11 @@
       <c r="I30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1936,19 +2260,19 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>8.9</v>
+        <v>7.9</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H31">
         <v>2.4900000000000002</v>
@@ -1956,8 +2280,11 @@
       <c r="I31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1968,16 +2295,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H32">
         <v>2.6</v>
@@ -1985,8 +2312,11 @@
       <c r="I32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1997,16 +2327,16 @@
         <v>8.9</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H33">
         <v>2.33</v>
@@ -2014,8 +2344,11 @@
       <c r="I33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2026,16 +2359,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H34">
         <v>1.67</v>
@@ -2043,8 +2376,11 @@
       <c r="I34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2052,19 +2388,19 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G35" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H35">
         <v>1.61</v>
@@ -2072,8 +2408,11 @@
       <c r="I35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2084,16 +2423,16 @@
         <v>7.3</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H36">
         <v>1.63</v>
@@ -2101,8 +2440,11 @@
       <c r="I36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2113,16 +2455,16 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H37">
         <v>1.32</v>
@@ -2130,8 +2472,11 @@
       <c r="I37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2142,16 +2487,16 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H38">
         <v>1.55</v>
@@ -2159,8 +2504,11 @@
       <c r="I38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2171,16 +2519,16 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E39" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H39">
         <v>1.34</v>
@@ -2188,8 +2536,11 @@
       <c r="I39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2197,19 +2548,19 @@
         <v>8</v>
       </c>
       <c r="C40">
-        <v>9.4</v>
+        <v>9.5</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H40">
         <v>1.26</v>
@@ -2217,8 +2568,11 @@
       <c r="I40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2229,16 +2583,16 @@
         <v>7.7</v>
       </c>
       <c r="D41" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E41" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F41" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H41">
         <v>1.22</v>
@@ -2246,8 +2600,11 @@
       <c r="I41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2255,19 +2612,19 @@
         <v>10</v>
       </c>
       <c r="C42">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H42">
         <v>1.3</v>
@@ -2275,8 +2632,11 @@
       <c r="I42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2287,16 +2647,16 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G43" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H43">
         <v>1.3</v>
@@ -2304,8 +2664,11 @@
       <c r="I43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2316,16 +2679,16 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H44">
         <v>1.1599999999999999</v>
@@ -2333,8 +2696,11 @@
       <c r="I44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2345,16 +2711,16 @@
         <v>7.8</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E45" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F45" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H45">
         <v>1.01</v>
@@ -2362,8 +2728,11 @@
       <c r="I45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2374,16 +2743,16 @@
         <v>5.7</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H46">
         <v>0.96</v>
@@ -2391,8 +2760,11 @@
       <c r="I46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2403,16 +2775,16 @@
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E47" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G47" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H47">
         <v>0.78</v>
@@ -2420,8 +2792,11 @@
       <c r="I47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>5</v>
       </c>
@@ -2432,16 +2807,16 @@
         <v>7.1</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E48" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H48">
         <v>0.93</v>
@@ -2449,8 +2824,11 @@
       <c r="I48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>5</v>
       </c>
@@ -2458,19 +2836,19 @@
         <v>7</v>
       </c>
       <c r="C49">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F49" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H49">
         <v>0.82</v>
@@ -2478,8 +2856,11 @@
       <c r="I49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2490,16 +2871,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E50" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F50" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G50" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H50">
         <v>0.83</v>
@@ -2507,8 +2888,11 @@
       <c r="I50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2516,19 +2900,19 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D51" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F51" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G51" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H51">
         <v>0.91</v>
@@ -2536,8 +2920,11 @@
       <c r="I51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2545,19 +2932,19 @@
         <v>10</v>
       </c>
       <c r="C52">
-        <v>9.4</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D52" t="s">
+        <v>156</v>
+      </c>
+      <c r="E52" t="s">
+        <v>105</v>
+      </c>
+      <c r="F52" t="s">
+        <v>157</v>
+      </c>
+      <c r="G52" t="s">
         <v>155</v>
-      </c>
-      <c r="E52" t="s">
-        <v>104</v>
-      </c>
-      <c r="F52" t="s">
-        <v>156</v>
-      </c>
-      <c r="G52" t="s">
-        <v>154</v>
       </c>
       <c r="H52">
         <v>0.94</v>
@@ -2565,8 +2952,11 @@
       <c r="I52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2574,19 +2964,19 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>8.8000000000000007</v>
+        <v>8.5</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F53" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G53" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H53">
         <v>0.66</v>
@@ -2594,8 +2984,11 @@
       <c r="I53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2603,19 +2996,19 @@
         <v>2</v>
       </c>
       <c r="C54">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="D54" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E54" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G54" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H54">
         <v>0.6</v>
@@ -2623,8 +3016,11 @@
       <c r="I54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2632,19 +3028,19 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
       <c r="D55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E55" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F55" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G55" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H55">
         <v>0.55000000000000004</v>
@@ -2652,8 +3048,11 @@
       <c r="I55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>6</v>
       </c>
@@ -2661,19 +3060,19 @@
         <v>4</v>
       </c>
       <c r="C56">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
       <c r="D56" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F56" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H56">
         <v>0.6</v>
@@ -2681,8 +3080,11 @@
       <c r="I56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>6</v>
       </c>
@@ -2690,19 +3092,19 @@
         <v>5</v>
       </c>
       <c r="C57">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D57" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F57" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G57" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H57">
         <v>0.57999999999999996</v>
@@ -2710,8 +3112,11 @@
       <c r="I57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>6</v>
       </c>
@@ -2719,19 +3124,19 @@
         <v>6</v>
       </c>
       <c r="C58">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E58" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F58" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G58" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H58">
         <v>0.54</v>
@@ -2739,8 +3144,11 @@
       <c r="I58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2748,19 +3156,19 @@
         <v>7</v>
       </c>
       <c r="C59">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="D59" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E59" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F59" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G59" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H59">
         <v>0.51</v>
@@ -2768,8 +3176,11 @@
       <c r="I59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>6</v>
       </c>
@@ -2780,16 +3191,16 @@
         <v>8.4</v>
       </c>
       <c r="D60" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E60" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F60" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G60" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H60">
         <v>0.53</v>
@@ -2800,8 +3211,11 @@
       <c r="J60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>6</v>
       </c>
@@ -2809,19 +3223,19 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>7.6</v>
+        <v>7.4</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E61" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F61" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G61" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H61">
         <v>0.53</v>
@@ -2832,8 +3246,11 @@
       <c r="J61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>6</v>
       </c>
@@ -2841,19 +3258,19 @@
         <v>10</v>
       </c>
       <c r="C62">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F62" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G62" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H62">
         <v>0.49</v>
@@ -2864,8 +3281,11 @@
       <c r="J62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="K62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63">
         <v>7</v>
       </c>
@@ -2873,19 +3293,19 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="D63" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E63" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F63" t="s">
-        <v>140</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>182</v>
+        <v>141</v>
+      </c>
+      <c r="G63" t="s">
+        <v>183</v>
       </c>
       <c r="H63">
         <v>0.42</v>
@@ -2893,8 +3313,11 @@
       <c r="I63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="K63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64">
         <v>7</v>
       </c>
@@ -2902,19 +3325,19 @@
         <v>2</v>
       </c>
       <c r="C64">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="D64" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E64" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F64" t="s">
-        <v>184</v>
-      </c>
-      <c r="G64" s="2" t="s">
         <v>185</v>
+      </c>
+      <c r="G64" t="s">
+        <v>186</v>
       </c>
       <c r="H64">
         <v>0.47</v>
@@ -2922,8 +3345,11 @@
       <c r="I64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="K64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>7</v>
       </c>
@@ -2934,16 +3360,16 @@
         <v>6.8</v>
       </c>
       <c r="D65" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F65" t="s">
-        <v>63</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>187</v>
+        <v>64</v>
+      </c>
+      <c r="G65" t="s">
+        <v>188</v>
       </c>
       <c r="H65">
         <v>0.36</v>
@@ -2951,8 +3377,11 @@
       <c r="I65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="28.5">
+      <c r="K65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>7</v>
       </c>
@@ -2963,16 +3392,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D66" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E66" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>167</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>189</v>
+        <v>168</v>
+      </c>
+      <c r="G66" t="s">
+        <v>190</v>
       </c>
       <c r="H66">
         <v>0.44</v>
@@ -2980,8 +3409,11 @@
       <c r="I66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="28.5">
+      <c r="K66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>7</v>
       </c>
@@ -2992,16 +3424,16 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D67" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F67" t="s">
-        <v>184</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
+      </c>
+      <c r="G67" t="s">
+        <v>192</v>
       </c>
       <c r="H67">
         <v>0.46</v>
@@ -3009,8 +3441,11 @@
       <c r="I67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="28.5">
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>7</v>
       </c>
@@ -3018,19 +3453,19 @@
         <v>6</v>
       </c>
       <c r="C68">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="D68" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F68" t="s">
-        <v>193</v>
-      </c>
-      <c r="G68" s="1" t="s">
         <v>194</v>
+      </c>
+      <c r="G68" t="s">
+        <v>195</v>
       </c>
       <c r="H68">
         <v>0.4</v>
@@ -3038,8 +3473,11 @@
       <c r="I68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="28.5">
+      <c r="K68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69">
         <v>7</v>
       </c>
@@ -3047,19 +3485,19 @@
         <v>7</v>
       </c>
       <c r="C69">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="D69" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E69" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F69" t="s">
-        <v>196</v>
-      </c>
-      <c r="G69" s="1" t="s">
         <v>197</v>
+      </c>
+      <c r="G69" t="s">
+        <v>198</v>
       </c>
       <c r="H69">
         <v>0.49</v>
@@ -3067,8 +3505,11 @@
       <c r="I69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="28.5">
+      <c r="K69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70">
         <v>7</v>
       </c>
@@ -3079,16 +3520,16 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D70" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E70" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F70" t="s">
-        <v>137</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>199</v>
+        <v>138</v>
+      </c>
+      <c r="G70" t="s">
+        <v>200</v>
       </c>
       <c r="H70">
         <v>0.38</v>
@@ -3096,8 +3537,11 @@
       <c r="I70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="28.5">
+      <c r="K70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71">
         <v>7</v>
       </c>
@@ -3105,19 +3549,19 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="D71" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E71" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F71" t="s">
-        <v>201</v>
-      </c>
-      <c r="G71" s="1" t="s">
         <v>202</v>
+      </c>
+      <c r="G71" t="s">
+        <v>203</v>
       </c>
       <c r="H71">
         <v>0.28999999999999998</v>
@@ -3125,8 +3569,11 @@
       <c r="I71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="28.5">
+      <c r="K71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72">
         <v>7</v>
       </c>
@@ -3137,18 +3584,335 @@
         <v>9.4</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E72" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F72" t="s">
-        <v>167</v>
-      </c>
-      <c r="G72" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G72" t="s">
+        <v>206</v>
+      </c>
+      <c r="H72">
+        <v>0.45</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>8</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D73" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73" t="s">
+        <v>175</v>
+      </c>
+      <c r="F73" t="s">
+        <v>208</v>
+      </c>
+      <c r="G73" t="s">
+        <v>209</v>
+      </c>
+      <c r="H73">
+        <v>0.3</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74">
+        <v>8</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
+        <v>210</v>
+      </c>
+      <c r="E74" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74" t="s">
+        <v>180</v>
+      </c>
+      <c r="G74" t="s">
+        <v>211</v>
+      </c>
+      <c r="H74">
+        <v>0.47</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75">
+        <v>8</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="C75">
+        <v>7.9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>212</v>
+      </c>
+      <c r="E75" t="s">
+        <v>213</v>
+      </c>
+      <c r="F75" t="s">
+        <v>214</v>
+      </c>
+      <c r="G75" t="s">
+        <v>215</v>
+      </c>
+      <c r="H75">
+        <v>0.33</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76">
+        <v>8</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <v>6.3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>216</v>
+      </c>
+      <c r="E76" t="s">
+        <v>163</v>
+      </c>
+      <c r="F76" t="s">
+        <v>168</v>
+      </c>
+      <c r="G76" t="s">
+        <v>217</v>
+      </c>
+      <c r="H76">
+        <v>0.38</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>8</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>218</v>
+      </c>
+      <c r="E77" t="s">
+        <v>175</v>
+      </c>
+      <c r="F77" t="s">
+        <v>141</v>
+      </c>
+      <c r="G77" t="s">
+        <v>219</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78">
+        <v>8</v>
+      </c>
+      <c r="B78">
+        <v>6</v>
+      </c>
+      <c r="C78">
+        <v>7.4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>220</v>
+      </c>
+      <c r="E78" t="s">
         <v>205</v>
       </c>
-      <c r="I72">
+      <c r="F78" t="s">
+        <v>221</v>
+      </c>
+      <c r="G78" t="s">
+        <v>222</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79">
+        <v>6.8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>223</v>
+      </c>
+      <c r="E79" t="s">
+        <v>163</v>
+      </c>
+      <c r="F79" t="s">
+        <v>138</v>
+      </c>
+      <c r="G79" t="s">
+        <v>224</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80">
+        <v>8</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+      <c r="C80">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>225</v>
+      </c>
+      <c r="E80" t="s">
+        <v>175</v>
+      </c>
+      <c r="F80" t="s">
+        <v>185</v>
+      </c>
+      <c r="G80" t="s">
+        <v>226</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>9</v>
+      </c>
+      <c r="C81">
+        <v>6.7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>227</v>
+      </c>
+      <c r="E81" t="s">
+        <v>205</v>
+      </c>
+      <c r="F81" t="s">
+        <v>228</v>
+      </c>
+      <c r="G81" t="s">
+        <v>229</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82">
+        <v>8</v>
+      </c>
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>230</v>
+      </c>
+      <c r="E82" t="s">
+        <v>213</v>
+      </c>
+      <c r="F82" t="s">
+        <v>185</v>
+      </c>
+      <c r="G82" t="s">
+        <v>231</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="K82">
         <v>0</v>
       </c>
     </row>
@@ -3156,4 +3920,317 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A528112A-D720-407B-B574-CCF3CECC318A}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H2:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="73.5">
+      <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60">
+      <c r="A2" s="3">
+        <v>72</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="3">
+        <v>73</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="104.25">
+      <c r="A4" s="3">
+        <v>74</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="74.25">
+      <c r="A5" s="3">
+        <v>75</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60">
+      <c r="A6" s="3">
+        <v>76</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="104.25">
+      <c r="A7" s="3">
+        <v>77</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45">
+      <c r="A8" s="3">
+        <v>78</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="89.25">
+      <c r="A9" s="3">
+        <v>79</v>
+      </c>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30.75">
+      <c r="A10" s="3">
+        <v>80</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="89.25">
+      <c r="A11" s="3">
+        <v>81</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1" location="cite_note-TFC-8" xr:uid="{145CAF88-196D-401C-B33A-F805379FA36F}"/>
+    <hyperlink ref="G1" r:id="rId2" location="cite_note-copy-30" xr:uid="{3B3C4819-F9E2-4644-80A0-5C1D5AA5C938}"/>
+    <hyperlink ref="H2" r:id="rId3" location="cite_note-86" xr:uid="{DD8C7B76-7890-4F37-9FB2-D50CE532A891}"/>
+    <hyperlink ref="H3" r:id="rId4" location="cite_note-87" xr:uid="{DE7D1843-71C7-44DA-8395-97F1834967B6}"/>
+    <hyperlink ref="H4" r:id="rId5" location="cite_note-88" xr:uid="{868001F3-C489-4F4C-928E-6F78FEB136E3}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{AD941798-B8B8-4B77-9386-F03222EDBBF7}"/>
+    <hyperlink ref="H5" r:id="rId7" location="cite_note-89" xr:uid="{5042619A-3E82-49F3-A804-D0AAD3332535}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{A9A9F6AF-0DA5-4949-B88F-116D855DCE70}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{414605C5-5E6F-47D7-89A0-0C5821892861}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{F013F4FD-7DD3-438E-B9D0-0F300D69F9D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>